<commit_message>
[assets] minor correction in ORB-v1.0
Use same example string as in NRB-v5.0 and NRB-v5.5 to avoid detection as difference:
- [1.6.3] `[format “2022-08-22T00:00:00.000000Z”]` -> `[format “2019-06-06T00:00:00.000000Z”]`
</commit_message>
<xml_diff>
--- a/assets/orb/CARD_METADATA-spec_ORB-v1.0.xlsx
+++ b/assets/orb/CARD_METADATA-spec_ORB-v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akerosenqvist/Library/Mobile Documents/com~apple~CloudDocs/iCloud Docs/CEOS/LSI-VC/CARD4L/@CARD4L PFSs DRAFTS/Ocean Radar Backscatter (ORB)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcowo/Documents/pypypy/ceos-ard-spec-tables/assets/orb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF613B7-AD3C-A245-B456-7D93256905A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE7B291-F2F5-9549-A827-1553A6102149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="28240" windowHeight="17500" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="33500" windowHeight="21580" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1st page" sheetId="5" r:id="rId1"/>
@@ -1263,9 +1263,6 @@
   </si>
   <si>
     <t xml:space="preserve"> type="Ocean Radar Backscatter",  version="1.0" *</t>
-  </si>
-  <si>
-    <t>[format “2022-08-22T00:00:00.000000Z”]</t>
   </si>
   <si>
     <t xml:space="preserve"> units="dB", type =["Beta0", "Sigma0"]</t>
@@ -1589,6 +1586,9 @@
   </si>
   <si>
     <t>29.09.2022</t>
+  </si>
+  <si>
+    <t>[format “2019-06-06T00:00:00.000000Z”]</t>
   </si>
 </sst>
 </file>
@@ -2924,12 +2924,42 @@
     <xf numFmtId="14" fontId="16" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2939,78 +2969,51 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3020,37 +3023,34 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3469,7 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3483,12 +3483,12 @@
       <c r="C2" s="11"/>
       <c r="D2" s="14"/>
       <c r="E2" s="145" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F2" s="146"/>
       <c r="G2" s="147"/>
       <c r="H2" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I2" s="155"/>
       <c r="J2" s="156"/>
@@ -3588,13 +3588,13 @@
       </c>
       <c r="D15" s="166"/>
       <c r="E15" s="143" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F15" s="143"/>
       <c r="G15" s="143"/>
       <c r="H15" s="143"/>
       <c r="I15" s="143" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J15" s="144"/>
     </row>
@@ -3603,17 +3603,17 @@
         <v>294</v>
       </c>
       <c r="C16" s="138" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D16" s="139"/>
       <c r="E16" s="140" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F16" s="141"/>
       <c r="G16" s="141"/>
       <c r="H16" s="142"/>
       <c r="I16" s="143" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J16" s="144"/>
     </row>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="20" spans="2:2" s="38" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B20" s="99" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="2:2" s="38" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
@@ -3666,7 +3666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:PL250"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3682,19 +3684,19 @@
     </row>
     <row r="2" spans="1:6" s="39" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="189" t="s">
+      <c r="C3" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="189" t="s">
+      <c r="D3" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="189" t="s">
+      <c r="E3" s="173" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -3702,23 +3704,23 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="190"/>
-      <c r="B4" s="194"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
+      <c r="A4" s="174"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="174"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="167">
+      <c r="A5" s="175">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B5" s="167" t="s">
+      <c r="B5" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="180" t="s">
         <v>137</v>
       </c>
       <c r="D5" s="23"/>
@@ -3726,21 +3728,21 @@
       <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="169"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="171"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="181"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="167">
+      <c r="A7" s="175">
         <v>1.2</v>
       </c>
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="177" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="170" t="s">
+      <c r="C7" s="180" t="s">
         <v>137</v>
       </c>
       <c r="D7" s="23"/>
@@ -3748,18 +3750,18 @@
       <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="168"/>
-      <c r="B8" s="173"/>
-      <c r="C8" s="171"/>
+      <c r="A8" s="176"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="181"/>
       <c r="D8" s="26"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="167">
+      <c r="A9" s="175">
         <v>1.3</v>
       </c>
-      <c r="B9" s="167" t="s">
+      <c r="B9" s="175" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3"/>
@@ -3768,8 +3770,8 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="168"/>
-      <c r="B10" s="168"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
@@ -3780,8 +3782,8 @@
       <c r="F10" s="51"/>
     </row>
     <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="169"/>
-      <c r="B11" s="169"/>
+      <c r="A11" s="179"/>
+      <c r="B11" s="179"/>
       <c r="C11" s="29"/>
       <c r="D11" s="30"/>
       <c r="E11" s="52" t="s">
@@ -3790,10 +3792,10 @@
       <c r="F11" s="53"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="167">
+      <c r="A12" s="175">
         <v>1.4</v>
       </c>
-      <c r="B12" s="167" t="s">
+      <c r="B12" s="175" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3"/>
@@ -3802,8 +3804,8 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="169"/>
-      <c r="B13" s="169"/>
+      <c r="A13" s="179"/>
+      <c r="B13" s="179"/>
       <c r="C13" s="29" t="s">
         <v>12</v>
       </c>
@@ -3816,10 +3818,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="167">
+      <c r="A14" s="175">
         <v>1.5</v>
       </c>
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="175" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="3"/>
@@ -3828,8 +3830,8 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="168"/>
-      <c r="B15" s="168"/>
+      <c r="A15" s="176"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="3" t="s">
         <v>113</v>
       </c>
@@ -3838,8 +3840,8 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="168"/>
-      <c r="B16" s="168"/>
+      <c r="A16" s="176"/>
+      <c r="B16" s="176"/>
       <c r="C16" s="3" t="s">
         <v>114</v>
       </c>
@@ -3850,8 +3852,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="168"/>
-      <c r="B17" s="168"/>
+      <c r="A17" s="176"/>
+      <c r="B17" s="176"/>
       <c r="C17" s="3" t="s">
         <v>212</v>
       </c>
@@ -3862,8 +3864,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="169"/>
-      <c r="B18" s="169"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="179"/>
       <c r="C18" s="30" t="s">
         <v>213</v>
       </c>
@@ -3874,10 +3876,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="167">
+      <c r="A19" s="175">
         <v>1.6</v>
       </c>
-      <c r="B19" s="167" t="s">
+      <c r="B19" s="175" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
@@ -3886,8 +3888,8 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="168"/>
-      <c r="B20" s="168"/>
+      <c r="A20" s="176"/>
+      <c r="B20" s="176"/>
       <c r="C20" s="35" t="s">
         <v>236</v>
       </c>
@@ -3900,10 +3902,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="167" t="s">
+      <c r="A21" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="167" t="s">
+      <c r="B21" s="175" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -3916,8 +3918,8 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="168"/>
-      <c r="B22" s="168"/>
+      <c r="A22" s="176"/>
+      <c r="B22" s="176"/>
       <c r="C22" s="3" t="s">
         <v>75</v>
       </c>
@@ -3930,18 +3932,18 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="169"/>
-      <c r="B23" s="169"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="179"/>
       <c r="C23" s="56"/>
       <c r="D23" s="30"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="167" t="s">
+      <c r="A24" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="167" t="s">
+      <c r="B24" s="175" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="3"/>
@@ -3950,8 +3952,8 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="168"/>
-      <c r="B25" s="168"/>
+      <c r="A25" s="176"/>
+      <c r="B25" s="176"/>
       <c r="C25" s="3" t="s">
         <v>18</v>
       </c>
@@ -3962,8 +3964,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="168"/>
-      <c r="B26" s="168"/>
+      <c r="A26" s="176"/>
+      <c r="B26" s="176"/>
       <c r="C26" s="3" t="s">
         <v>238</v>
       </c>
@@ -3974,8 +3976,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="168"/>
-      <c r="B27" s="168"/>
+      <c r="A27" s="176"/>
+      <c r="B27" s="176"/>
       <c r="C27" s="3"/>
       <c r="D27" s="35" t="s">
         <v>237</v>
@@ -3988,10 +3990,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="167" t="s">
+      <c r="A28" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="172" t="s">
+      <c r="B28" s="177" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="31"/>
@@ -4000,8 +4002,8 @@
       <c r="F28" s="33"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="168"/>
-      <c r="B29" s="173"/>
+      <c r="A29" s="176"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="60" t="s">
         <v>211</v>
       </c>
@@ -4010,8 +4012,8 @@
       <c r="F29" s="61"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="168"/>
-      <c r="B30" s="173"/>
+      <c r="A30" s="176"/>
+      <c r="B30" s="178"/>
       <c r="C30" s="60" t="s">
         <v>190</v>
       </c>
@@ -4022,8 +4024,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="168"/>
-      <c r="B31" s="173"/>
+      <c r="A31" s="176"/>
+      <c r="B31" s="178"/>
       <c r="C31" s="60" t="s">
         <v>191</v>
       </c>
@@ -4034,20 +4036,20 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="169"/>
-      <c r="B32" s="174"/>
+      <c r="A32" s="179"/>
+      <c r="B32" s="194"/>
       <c r="C32" s="62"/>
       <c r="D32" s="35"/>
       <c r="E32" s="55"/>
       <c r="F32" s="37" t="s">
-        <v>296</v>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="167" t="s">
+      <c r="A33" s="175" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="167" t="s">
+      <c r="B33" s="175" t="s">
         <v>126</v>
       </c>
       <c r="C33" s="63"/>
@@ -4056,8 +4058,8 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="168"/>
-      <c r="B34" s="168"/>
+      <c r="A34" s="176"/>
+      <c r="B34" s="176"/>
       <c r="C34" s="3" t="s">
         <v>199</v>
       </c>
@@ -4066,8 +4068,8 @@
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="168"/>
-      <c r="B35" s="168"/>
+      <c r="A35" s="176"/>
+      <c r="B35" s="176"/>
       <c r="C35" s="3" t="s">
         <v>76</v>
       </c>
@@ -4078,8 +4080,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="168"/>
-      <c r="B36" s="168"/>
+      <c r="A36" s="176"/>
+      <c r="B36" s="176"/>
       <c r="C36" s="3" t="s">
         <v>77</v>
       </c>
@@ -4092,8 +4094,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="168"/>
-      <c r="B37" s="168"/>
+      <c r="A37" s="176"/>
+      <c r="B37" s="176"/>
       <c r="C37" s="3" t="s">
         <v>78</v>
       </c>
@@ -4104,8 +4106,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="168"/>
-      <c r="B38" s="168"/>
+      <c r="A38" s="176"/>
+      <c r="B38" s="176"/>
       <c r="C38" s="3" t="s">
         <v>79</v>
       </c>
@@ -4116,8 +4118,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="168"/>
-      <c r="B39" s="168"/>
+      <c r="A39" s="176"/>
+      <c r="B39" s="176"/>
       <c r="C39" s="3" t="s">
         <v>110</v>
       </c>
@@ -4128,8 +4130,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="169"/>
-      <c r="B40" s="169"/>
+      <c r="A40" s="179"/>
+      <c r="B40" s="179"/>
       <c r="C40" s="29" t="s">
         <v>80</v>
       </c>
@@ -4140,10 +4142,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="167" t="s">
+      <c r="A41" s="175" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="167" t="s">
+      <c r="B41" s="175" t="s">
         <v>20</v>
       </c>
       <c r="C41" s="3"/>
@@ -4152,8 +4154,8 @@
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="168"/>
-      <c r="B42" s="168"/>
+      <c r="A42" s="176"/>
+      <c r="B42" s="176"/>
       <c r="C42" s="3" t="s">
         <v>21</v>
       </c>
@@ -4162,8 +4164,8 @@
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="168"/>
-      <c r="B43" s="168"/>
+      <c r="A43" s="176"/>
+      <c r="B43" s="176"/>
       <c r="C43" s="3" t="s">
         <v>81</v>
       </c>
@@ -4174,8 +4176,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="168"/>
-      <c r="B44" s="168"/>
+      <c r="A44" s="176"/>
+      <c r="B44" s="176"/>
       <c r="C44" s="3" t="s">
         <v>239</v>
       </c>
@@ -4186,8 +4188,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="168"/>
-      <c r="B45" s="168"/>
+      <c r="A45" s="176"/>
+      <c r="B45" s="176"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
         <v>243</v>
@@ -4198,8 +4200,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A46" s="168"/>
-      <c r="B46" s="168"/>
+      <c r="A46" s="176"/>
+      <c r="B46" s="176"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
         <v>263</v>
@@ -4210,8 +4212,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="168"/>
-      <c r="B47" s="168"/>
+      <c r="A47" s="176"/>
+      <c r="B47" s="176"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
         <v>273</v>
@@ -4220,8 +4222,8 @@
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="168"/>
-      <c r="B48" s="168"/>
+      <c r="A48" s="176"/>
+      <c r="B48" s="176"/>
       <c r="C48" s="3"/>
       <c r="D48" s="90" t="s">
         <v>262</v>
@@ -4232,8 +4234,8 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="168"/>
-      <c r="B49" s="168"/>
+      <c r="A49" s="176"/>
+      <c r="B49" s="176"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
         <v>255</v>
@@ -4246,8 +4248,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="168"/>
-      <c r="B50" s="168"/>
+      <c r="A50" s="176"/>
+      <c r="B50" s="176"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
         <v>256</v>
@@ -4260,8 +4262,8 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="168"/>
-      <c r="B51" s="168"/>
+      <c r="A51" s="176"/>
+      <c r="B51" s="176"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
         <v>257</v>
@@ -4274,8 +4276,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="168"/>
-      <c r="B52" s="168"/>
+      <c r="A52" s="176"/>
+      <c r="B52" s="176"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
         <v>258</v>
@@ -4288,8 +4290,8 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="168"/>
-      <c r="B53" s="168"/>
+      <c r="A53" s="176"/>
+      <c r="B53" s="176"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
         <v>259</v>
@@ -4302,8 +4304,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="168"/>
-      <c r="B54" s="168"/>
+      <c r="A54" s="176"/>
+      <c r="B54" s="176"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
         <v>260</v>
@@ -4316,8 +4318,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="168"/>
-      <c r="B55" s="168"/>
+      <c r="A55" s="176"/>
+      <c r="B55" s="176"/>
       <c r="C55" s="4"/>
       <c r="D55" s="3" t="s">
         <v>82</v>
@@ -4330,8 +4332,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="169"/>
-      <c r="B56" s="169"/>
+      <c r="A56" s="179"/>
+      <c r="B56" s="179"/>
       <c r="C56" s="56"/>
       <c r="D56" s="3" t="s">
         <v>83</v>
@@ -4344,10 +4346,10 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="167" t="s">
+      <c r="A57" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="167" t="s">
+      <c r="B57" s="175" t="s">
         <v>22</v>
       </c>
       <c r="C57" s="64"/>
@@ -4356,8 +4358,8 @@
       <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="168"/>
-      <c r="B58" s="168"/>
+      <c r="A58" s="176"/>
+      <c r="B58" s="176"/>
       <c r="C58" s="40" t="s">
         <v>23</v>
       </c>
@@ -4368,8 +4370,8 @@
       <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="168"/>
-      <c r="B59" s="168"/>
+      <c r="A59" s="176"/>
+      <c r="B59" s="176"/>
       <c r="C59" s="40" t="s">
         <v>84</v>
       </c>
@@ -4380,8 +4382,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="168"/>
-      <c r="B60" s="168"/>
+      <c r="A60" s="176"/>
+      <c r="B60" s="176"/>
       <c r="C60" s="40" t="s">
         <v>85</v>
       </c>
@@ -4392,8 +4394,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="168"/>
-      <c r="B61" s="168"/>
+      <c r="A61" s="176"/>
+      <c r="B61" s="176"/>
       <c r="C61" s="40" t="s">
         <v>86</v>
       </c>
@@ -4404,8 +4406,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="168"/>
-      <c r="B62" s="168"/>
+      <c r="A62" s="176"/>
+      <c r="B62" s="176"/>
       <c r="C62" s="40" t="s">
         <v>87</v>
       </c>
@@ -4416,8 +4418,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="168"/>
-      <c r="B63" s="168"/>
+      <c r="A63" s="176"/>
+      <c r="B63" s="176"/>
       <c r="C63" s="40" t="s">
         <v>88</v>
       </c>
@@ -4428,8 +4430,8 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="168"/>
-      <c r="B64" s="168"/>
+      <c r="A64" s="176"/>
+      <c r="B64" s="176"/>
       <c r="C64" s="40" t="s">
         <v>210</v>
       </c>
@@ -4440,8 +4442,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="168"/>
-      <c r="B65" s="168"/>
+      <c r="A65" s="176"/>
+      <c r="B65" s="176"/>
       <c r="C65" s="40"/>
       <c r="D65" s="67" t="s">
         <v>185</v>
@@ -4452,8 +4454,8 @@
       <c r="F65" s="122"/>
     </row>
     <row r="66" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A66" s="168"/>
-      <c r="B66" s="168"/>
+      <c r="A66" s="176"/>
+      <c r="B66" s="176"/>
       <c r="C66" s="40"/>
       <c r="D66" s="67" t="s">
         <v>216</v>
@@ -4466,8 +4468,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="168"/>
-      <c r="B67" s="168"/>
+      <c r="A67" s="176"/>
+      <c r="B67" s="176"/>
       <c r="C67" s="40" t="s">
         <v>89</v>
       </c>
@@ -4480,8 +4482,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="168"/>
-      <c r="B68" s="168"/>
+      <c r="A68" s="176"/>
+      <c r="B68" s="176"/>
       <c r="C68" s="40"/>
       <c r="D68" s="67" t="s">
         <v>186</v>
@@ -4492,8 +4494,8 @@
       <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A69" s="168"/>
-      <c r="B69" s="168"/>
+      <c r="A69" s="176"/>
+      <c r="B69" s="176"/>
       <c r="C69" s="40"/>
       <c r="D69" s="67" t="s">
         <v>216</v>
@@ -4506,8 +4508,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="168"/>
-      <c r="B70" s="168"/>
+      <c r="A70" s="176"/>
+      <c r="B70" s="176"/>
       <c r="C70" s="69"/>
       <c r="D70" s="70" t="s">
         <v>111</v>
@@ -4518,10 +4520,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="167" t="s">
+      <c r="A71" s="175" t="s">
         <v>45</v>
       </c>
-      <c r="B71" s="167" t="s">
+      <c r="B71" s="175" t="s">
         <v>24</v>
       </c>
       <c r="C71" s="4"/>
@@ -4530,8 +4532,8 @@
       <c r="F71" s="81"/>
     </row>
     <row r="72" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="168"/>
-      <c r="B72" s="168"/>
+      <c r="A72" s="176"/>
+      <c r="B72" s="176"/>
       <c r="C72" s="3" t="s">
         <v>188</v>
       </c>
@@ -4542,8 +4544,8 @@
       <c r="F72" s="51"/>
     </row>
     <row r="73" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="168"/>
-      <c r="B73" s="168"/>
+      <c r="A73" s="176"/>
+      <c r="B73" s="176"/>
       <c r="C73" s="3" t="s">
         <v>187</v>
       </c>
@@ -4554,8 +4556,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="168"/>
-      <c r="B74" s="168"/>
+      <c r="A74" s="176"/>
+      <c r="B74" s="176"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
         <v>287</v>
@@ -4568,8 +4570,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="168"/>
-      <c r="B75" s="168"/>
+      <c r="A75" s="176"/>
+      <c r="B75" s="176"/>
       <c r="C75" s="3"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
@@ -4578,8 +4580,8 @@
       <c r="F75" s="51"/>
     </row>
     <row r="76" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="168"/>
-      <c r="B76" s="168"/>
+      <c r="A76" s="176"/>
+      <c r="B76" s="176"/>
       <c r="C76" s="3" t="s">
         <v>90</v>
       </c>
@@ -4594,8 +4596,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="168"/>
-      <c r="B77" s="168"/>
+      <c r="A77" s="176"/>
+      <c r="B77" s="176"/>
       <c r="C77" s="3" t="s">
         <v>91</v>
       </c>
@@ -4608,8 +4610,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="168"/>
-      <c r="B78" s="168"/>
+      <c r="A78" s="176"/>
+      <c r="B78" s="176"/>
       <c r="C78" s="3" t="s">
         <v>92</v>
       </c>
@@ -4620,8 +4622,8 @@
       <c r="F78" s="51"/>
     </row>
     <row r="79" spans="1:6" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A79" s="168"/>
-      <c r="B79" s="168"/>
+      <c r="A79" s="176"/>
+      <c r="B79" s="176"/>
       <c r="C79" s="67" t="s">
         <v>216</v>
       </c>
@@ -4634,8 +4636,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="168"/>
-      <c r="B80" s="168"/>
+      <c r="A80" s="176"/>
+      <c r="B80" s="176"/>
       <c r="C80" s="3" t="s">
         <v>93</v>
       </c>
@@ -4646,8 +4648,8 @@
       <c r="F80" s="51"/>
     </row>
     <row r="81" spans="1:428" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A81" s="168"/>
-      <c r="B81" s="168"/>
+      <c r="A81" s="176"/>
+      <c r="B81" s="176"/>
       <c r="C81" s="67" t="s">
         <v>216</v>
       </c>
@@ -4660,8 +4662,8 @@
       </c>
     </row>
     <row r="82" spans="1:428" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="168"/>
-      <c r="B82" s="168"/>
+      <c r="A82" s="176"/>
+      <c r="B82" s="176"/>
       <c r="C82" s="74" t="s">
         <v>194</v>
       </c>
@@ -4674,8 +4676,8 @@
       </c>
     </row>
     <row r="83" spans="1:428" s="7" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="168"/>
-      <c r="B83" s="168"/>
+      <c r="A83" s="176"/>
+      <c r="B83" s="176"/>
       <c r="C83" s="3" t="s">
         <v>94</v>
       </c>
@@ -4688,10 +4690,10 @@
       </c>
     </row>
     <row r="84" spans="1:428" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="167" t="s">
+      <c r="A84" s="175" t="s">
         <v>48</v>
       </c>
-      <c r="B84" s="172" t="s">
+      <c r="B84" s="177" t="s">
         <v>25</v>
       </c>
       <c r="C84" s="31"/>
@@ -4700,8 +4702,8 @@
       <c r="F84" s="33"/>
     </row>
     <row r="85" spans="1:428" s="7" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="168"/>
-      <c r="B85" s="173"/>
+      <c r="A85" s="176"/>
+      <c r="B85" s="178"/>
       <c r="C85" s="34"/>
       <c r="D85" s="35" t="s">
         <v>241</v>
@@ -4714,10 +4716,10 @@
       </c>
     </row>
     <row r="86" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="167" t="s">
+      <c r="A86" s="175" t="s">
         <v>51</v>
       </c>
-      <c r="B86" s="167" t="s">
+      <c r="B86" s="175" t="s">
         <v>26</v>
       </c>
       <c r="C86" s="3"/>
@@ -4730,8 +4732,8 @@
       <c r="F86" s="4"/>
     </row>
     <row r="87" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="168"/>
-      <c r="B87" s="168"/>
+      <c r="A87" s="176"/>
+      <c r="B87" s="176"/>
       <c r="C87" s="3" t="s">
         <v>27</v>
       </c>
@@ -4742,20 +4744,20 @@
       <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="168"/>
-      <c r="B88" s="168"/>
+      <c r="A88" s="176"/>
+      <c r="B88" s="176"/>
       <c r="C88" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F88" s="4"/>
     </row>
     <row r="89" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="168"/>
-      <c r="B89" s="168"/>
+      <c r="A89" s="176"/>
+      <c r="B89" s="176"/>
       <c r="C89" s="3" t="s">
         <v>271</v>
       </c>
@@ -4768,8 +4770,8 @@
       </c>
     </row>
     <row r="90" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="168"/>
-      <c r="B90" s="168"/>
+      <c r="A90" s="176"/>
+      <c r="B90" s="176"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
         <v>240</v>
@@ -4780,8 +4782,8 @@
       </c>
     </row>
     <row r="91" spans="1:428" ht="48" x14ac:dyDescent="0.2">
-      <c r="A91" s="168"/>
-      <c r="B91" s="168"/>
+      <c r="A91" s="176"/>
+      <c r="B91" s="176"/>
       <c r="C91" s="3" t="s">
         <v>28</v>
       </c>
@@ -4796,8 +4798,8 @@
       </c>
     </row>
     <row r="92" spans="1:428" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="168"/>
-      <c r="B92" s="168"/>
+      <c r="A92" s="176"/>
+      <c r="B92" s="176"/>
       <c r="C92" s="3"/>
       <c r="D92" s="30" t="s">
         <v>96</v>
@@ -4810,10 +4812,10 @@
       </c>
     </row>
     <row r="93" spans="1:428" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="167" t="s">
+      <c r="A93" s="175" t="s">
         <v>274</v>
       </c>
-      <c r="B93" s="167" t="s">
+      <c r="B93" s="175" t="s">
         <v>275</v>
       </c>
       <c r="C93" s="54"/>
@@ -5193,8 +5195,8 @@
       <c r="PL93" s="7"/>
     </row>
     <row r="94" spans="1:428" ht="22.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="168"/>
-      <c r="B94" s="168"/>
+      <c r="A94" s="176"/>
+      <c r="B94" s="176"/>
       <c r="C94" s="30"/>
       <c r="D94" s="35" t="s">
         <v>277</v>
@@ -5574,10 +5576,10 @@
       <c r="PL94" s="7"/>
     </row>
     <row r="95" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="167" t="s">
+      <c r="A95" s="175" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="167" t="s">
+      <c r="B95" s="175" t="s">
         <v>29</v>
       </c>
       <c r="C95" s="54"/>
@@ -5588,8 +5590,8 @@
       <c r="F95" s="4"/>
     </row>
     <row r="96" spans="1:428" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="168"/>
-      <c r="B96" s="168"/>
+      <c r="A96" s="176"/>
+      <c r="B96" s="176"/>
       <c r="C96" s="50"/>
       <c r="D96" s="3" t="s">
         <v>278</v>
@@ -5602,8 +5604,8 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="169"/>
-      <c r="B97" s="169"/>
+      <c r="A97" s="179"/>
+      <c r="B97" s="179"/>
       <c r="C97" s="30"/>
       <c r="D97" s="29" t="s">
         <v>280</v>
@@ -5616,10 +5618,10 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="167" t="s">
+      <c r="A98" s="175" t="s">
         <v>116</v>
       </c>
-      <c r="B98" s="167" t="s">
+      <c r="B98" s="175" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="5"/>
@@ -5630,8 +5632,8 @@
       <c r="F98" s="4"/>
     </row>
     <row r="99" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="168"/>
-      <c r="B99" s="168"/>
+      <c r="A99" s="176"/>
+      <c r="B99" s="176"/>
       <c r="C99" s="55"/>
       <c r="D99" s="3" t="s">
         <v>279</v>
@@ -5642,11 +5644,11 @@
       </c>
     </row>
     <row r="100" spans="1:6" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="191">
+      <c r="A100" s="182">
         <v>1.7</v>
       </c>
-      <c r="B100" s="191" t="s">
-        <v>340</v>
+      <c r="B100" s="182" t="s">
+        <v>339</v>
       </c>
       <c r="C100" s="92"/>
       <c r="D100" s="93"/>
@@ -5656,10 +5658,10 @@
       <c r="F100" s="95"/>
     </row>
     <row r="101" spans="1:6" s="7" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="192"/>
-      <c r="B101" s="192"/>
+      <c r="A101" s="183"/>
+      <c r="B101" s="183"/>
       <c r="C101" s="35" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D101" s="96"/>
       <c r="E101" s="97"/>
@@ -5668,10 +5670,10 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="167" t="s">
+      <c r="A102" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="B102" s="167" t="s">
+      <c r="B102" s="175" t="s">
         <v>32</v>
       </c>
       <c r="C102" s="3"/>
@@ -5682,8 +5684,8 @@
       <c r="F102" s="4"/>
     </row>
     <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="168"/>
-      <c r="B103" s="168"/>
+      <c r="A103" s="176"/>
+      <c r="B103" s="176"/>
       <c r="C103" s="3" t="s">
         <v>33</v>
       </c>
@@ -5692,8 +5694,8 @@
       <c r="F103" s="4"/>
     </row>
     <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="168"/>
-      <c r="B104" s="168"/>
+      <c r="A104" s="176"/>
+      <c r="B104" s="176"/>
       <c r="C104" s="3" t="s">
         <v>84</v>
       </c>
@@ -5704,8 +5706,8 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="168"/>
-      <c r="B105" s="168"/>
+      <c r="A105" s="176"/>
+      <c r="B105" s="176"/>
       <c r="C105" s="3" t="s">
         <v>97</v>
       </c>
@@ -5716,8 +5718,8 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="168"/>
-      <c r="B106" s="168"/>
+      <c r="A106" s="176"/>
+      <c r="B106" s="176"/>
       <c r="C106" s="3" t="s">
         <v>86</v>
       </c>
@@ -5728,8 +5730,8 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="169"/>
-      <c r="B107" s="169"/>
+      <c r="A107" s="179"/>
+      <c r="B107" s="179"/>
       <c r="C107" s="29" t="s">
         <v>292</v>
       </c>
@@ -5742,10 +5744,10 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="167" t="s">
+      <c r="A108" s="175" t="s">
         <v>118</v>
       </c>
-      <c r="B108" s="167" t="s">
+      <c r="B108" s="175" t="s">
         <v>35</v>
       </c>
       <c r="C108" s="45"/>
@@ -5754,8 +5756,8 @@
       <c r="F108" s="4"/>
     </row>
     <row r="109" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="169"/>
-      <c r="B109" s="169"/>
+      <c r="A109" s="179"/>
+      <c r="B109" s="179"/>
       <c r="C109" s="47"/>
       <c r="D109" s="48" t="s">
         <v>204</v>
@@ -5768,10 +5770,10 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="167" t="s">
+      <c r="A110" s="175" t="s">
         <v>119</v>
       </c>
-      <c r="B110" s="167" t="s">
+      <c r="B110" s="175" t="s">
         <v>37</v>
       </c>
       <c r="C110" s="4"/>
@@ -5782,8 +5784,8 @@
       <c r="F110" s="4"/>
     </row>
     <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="168"/>
-      <c r="B111" s="168"/>
+      <c r="A111" s="176"/>
+      <c r="B111" s="176"/>
       <c r="C111" s="3" t="s">
         <v>38</v>
       </c>
@@ -5792,8 +5794,8 @@
       <c r="F111" s="4"/>
     </row>
     <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="168"/>
-      <c r="B112" s="168"/>
+      <c r="A112" s="176"/>
+      <c r="B112" s="176"/>
       <c r="C112" s="3" t="s">
         <v>98</v>
       </c>
@@ -5806,8 +5808,8 @@
       </c>
     </row>
     <row r="113" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="168"/>
-      <c r="B113" s="168"/>
+      <c r="A113" s="176"/>
+      <c r="B113" s="176"/>
       <c r="C113" s="35" t="s">
         <v>99</v>
       </c>
@@ -5820,11 +5822,11 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="167" t="s">
+      <c r="A114" s="175" t="s">
         <v>120</v>
       </c>
-      <c r="B114" s="167" t="s">
-        <v>298</v>
+      <c r="B114" s="175" t="s">
+        <v>297</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="123"/>
@@ -5834,11 +5836,11 @@
       <c r="F114" s="4"/>
     </row>
     <row r="115" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="168"/>
-      <c r="B115" s="168"/>
+      <c r="A115" s="176"/>
+      <c r="B115" s="176"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E115" s="51"/>
       <c r="F115" s="4" t="s">
@@ -5846,11 +5848,11 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="172" t="s">
+      <c r="A116" s="177" t="s">
         <v>121</v>
       </c>
-      <c r="B116" s="178" t="s">
-        <v>300</v>
+      <c r="B116" s="186" t="s">
+        <v>299</v>
       </c>
       <c r="C116" s="32"/>
       <c r="D116" s="59"/>
@@ -5860,21 +5862,21 @@
       <c r="F116" s="33"/>
     </row>
     <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="173"/>
-      <c r="B117" s="179"/>
+      <c r="A117" s="178"/>
+      <c r="B117" s="192"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E117" s="51"/>
       <c r="F117" s="61"/>
     </row>
     <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="173"/>
-      <c r="B118" s="179"/>
+      <c r="A118" s="178"/>
+      <c r="B118" s="192"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E118" s="51" t="s">
         <v>193</v>
@@ -5884,11 +5886,11 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="173"/>
-      <c r="B119" s="180"/>
+      <c r="A119" s="178"/>
+      <c r="B119" s="187"/>
       <c r="C119" s="35"/>
       <c r="D119" s="35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E119" s="55" t="s">
         <v>193</v>
@@ -5898,11 +5900,11 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="167" t="s">
+      <c r="A120" s="175" t="s">
         <v>122</v>
       </c>
-      <c r="B120" s="168" t="s">
-        <v>347</v>
+      <c r="B120" s="176" t="s">
+        <v>346</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="51"/>
@@ -5912,8 +5914,8 @@
       <c r="F120" s="4"/>
     </row>
     <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="168"/>
-      <c r="B121" s="168"/>
+      <c r="A121" s="176"/>
+      <c r="B121" s="176"/>
       <c r="C121" s="3" t="s">
         <v>40</v>
       </c>
@@ -5922,8 +5924,8 @@
       <c r="F121" s="4"/>
     </row>
     <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="168"/>
-      <c r="B122" s="168"/>
+      <c r="A122" s="176"/>
+      <c r="B122" s="176"/>
       <c r="C122" s="3" t="s">
         <v>41</v>
       </c>
@@ -5934,8 +5936,8 @@
       </c>
     </row>
     <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="168"/>
-      <c r="B123" s="168"/>
+      <c r="A123" s="176"/>
+      <c r="B123" s="176"/>
       <c r="C123" s="3" t="s">
         <v>100</v>
       </c>
@@ -5946,8 +5948,8 @@
       </c>
     </row>
     <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="168"/>
-      <c r="B124" s="168"/>
+      <c r="A124" s="176"/>
+      <c r="B124" s="176"/>
       <c r="C124" s="3" t="s">
         <v>53</v>
       </c>
@@ -5958,8 +5960,8 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="168"/>
-      <c r="B125" s="168"/>
+      <c r="A125" s="176"/>
+      <c r="B125" s="176"/>
       <c r="C125" s="3" t="s">
         <v>101</v>
       </c>
@@ -5970,8 +5972,8 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="169"/>
-      <c r="B126" s="169"/>
+      <c r="A126" s="179"/>
+      <c r="B126" s="179"/>
       <c r="C126" s="29" t="s">
         <v>42</v>
       </c>
@@ -5980,10 +5982,10 @@
       <c r="F126" s="56"/>
     </row>
     <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="175" t="s">
+      <c r="A127" s="190" t="s">
         <v>123</v>
       </c>
-      <c r="B127" s="175" t="s">
+      <c r="B127" s="190" t="s">
         <v>181</v>
       </c>
       <c r="C127" s="4"/>
@@ -5994,8 +5996,8 @@
       <c r="F127" s="4"/>
     </row>
     <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="176"/>
-      <c r="B128" s="176"/>
+      <c r="A128" s="191"/>
+      <c r="B128" s="191"/>
       <c r="C128" s="3" t="s">
         <v>184</v>
       </c>
@@ -6004,8 +6006,8 @@
       <c r="F128" s="4"/>
     </row>
     <row r="129" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A129" s="176"/>
-      <c r="B129" s="176"/>
+      <c r="A129" s="191"/>
+      <c r="B129" s="191"/>
       <c r="C129" s="3" t="s">
         <v>269</v>
       </c>
@@ -6018,8 +6020,8 @@
       </c>
     </row>
     <row r="130" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A130" s="176"/>
-      <c r="B130" s="176"/>
+      <c r="A130" s="191"/>
+      <c r="B130" s="191"/>
       <c r="C130" s="3" t="s">
         <v>270</v>
       </c>
@@ -6032,8 +6034,8 @@
       </c>
     </row>
     <row r="131" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="177"/>
-      <c r="B131" s="177"/>
+      <c r="A131" s="193"/>
+      <c r="B131" s="193"/>
       <c r="C131" s="29"/>
       <c r="D131" s="29" t="s">
         <v>183</v>
@@ -6046,10 +6048,10 @@
       </c>
     </row>
     <row r="132" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A132" s="175" t="s">
+      <c r="A132" s="190" t="s">
         <v>124</v>
       </c>
-      <c r="B132" s="175" t="s">
+      <c r="B132" s="190" t="s">
         <v>182</v>
       </c>
       <c r="C132" s="5"/>
@@ -6060,8 +6062,8 @@
       <c r="F132" s="80"/>
     </row>
     <row r="133" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="176"/>
-      <c r="B133" s="176"/>
+      <c r="A133" s="191"/>
+      <c r="B133" s="191"/>
       <c r="C133" s="50" t="s">
         <v>195</v>
       </c>
@@ -6074,8 +6076,8 @@
       </c>
     </row>
     <row r="134" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="176"/>
-      <c r="B134" s="176"/>
+      <c r="A134" s="191"/>
+      <c r="B134" s="191"/>
       <c r="C134" s="30"/>
       <c r="D134" s="53"/>
       <c r="E134" s="52" t="s">
@@ -6084,10 +6086,10 @@
       <c r="F134" s="52"/>
     </row>
     <row r="135" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="A135" s="167" t="s">
+      <c r="A135" s="175" t="s">
         <v>125</v>
       </c>
-      <c r="B135" s="167" t="s">
+      <c r="B135" s="175" t="s">
         <v>46</v>
       </c>
       <c r="C135" s="4"/>
@@ -6096,8 +6098,8 @@
       <c r="F135" s="4"/>
     </row>
     <row r="136" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136" s="168"/>
-      <c r="B136" s="168"/>
+      <c r="A136" s="176"/>
+      <c r="B136" s="176"/>
       <c r="C136" s="3" t="s">
         <v>47</v>
       </c>
@@ -6106,8 +6108,8 @@
       <c r="F136" s="4"/>
     </row>
     <row r="137" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="168"/>
-      <c r="B137" s="168"/>
+      <c r="A137" s="176"/>
+      <c r="B137" s="176"/>
       <c r="C137" s="3" t="s">
         <v>102</v>
       </c>
@@ -6118,8 +6120,8 @@
       </c>
     </row>
     <row r="138" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A138" s="168"/>
-      <c r="B138" s="168"/>
+      <c r="A138" s="176"/>
+      <c r="B138" s="176"/>
       <c r="C138" s="3" t="s">
         <v>103</v>
       </c>
@@ -6130,8 +6132,8 @@
       </c>
     </row>
     <row r="139" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A139" s="168"/>
-      <c r="B139" s="168"/>
+      <c r="A139" s="176"/>
+      <c r="B139" s="176"/>
       <c r="C139" s="3" t="s">
         <v>268</v>
       </c>
@@ -6144,8 +6146,8 @@
       </c>
     </row>
     <row r="140" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="168"/>
-      <c r="B140" s="168"/>
+      <c r="A140" s="176"/>
+      <c r="B140" s="176"/>
       <c r="C140" s="50" t="s">
         <v>267</v>
       </c>
@@ -6157,10 +6159,10 @@
       <c r="BG140"/>
     </row>
     <row r="141" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" s="178" t="s">
+      <c r="A141" s="186" t="s">
         <v>203</v>
       </c>
-      <c r="B141" s="187" t="s">
+      <c r="B141" s="188" t="s">
         <v>49</v>
       </c>
       <c r="C141" s="77"/>
@@ -6171,8 +6173,8 @@
       <c r="F141" s="33"/>
     </row>
     <row r="142" spans="1:59" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="180"/>
-      <c r="B142" s="188"/>
+      <c r="A142" s="187"/>
+      <c r="B142" s="189"/>
       <c r="C142" s="78" t="s">
         <v>50</v>
       </c>
@@ -6183,10 +6185,10 @@
       </c>
     </row>
     <row r="143" spans="1:59" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="181" t="s">
-        <v>304</v>
-      </c>
-      <c r="B143" s="184" t="s">
+      <c r="A143" s="167" t="s">
+        <v>303</v>
+      </c>
+      <c r="B143" s="170" t="s">
         <v>52</v>
       </c>
       <c r="C143" s="77"/>
@@ -6197,8 +6199,8 @@
       <c r="F143" s="33"/>
     </row>
     <row r="144" spans="1:59" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="182"/>
-      <c r="B144" s="185"/>
+      <c r="A144" s="168"/>
+      <c r="B144" s="171"/>
       <c r="C144" s="3" t="s">
         <v>266</v>
       </c>
@@ -6211,8 +6213,8 @@
       </c>
     </row>
     <row r="145" spans="1:59" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="183"/>
-      <c r="B145" s="186"/>
+      <c r="A145" s="169"/>
+      <c r="B145" s="172"/>
       <c r="C145" s="35" t="s">
         <v>266</v>
       </c>
@@ -6226,11 +6228,11 @@
       <c r="BG145"/>
     </row>
     <row r="146" spans="1:59" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="181" t="s">
+      <c r="A146" s="167" t="s">
+        <v>304</v>
+      </c>
+      <c r="B146" s="170" t="s">
         <v>305</v>
-      </c>
-      <c r="B146" s="184" t="s">
-        <v>306</v>
       </c>
       <c r="C146" s="32"/>
       <c r="D146" s="59"/>
@@ -6240,22 +6242,22 @@
       <c r="F146" s="33"/>
     </row>
     <row r="147" spans="1:59" ht="48" x14ac:dyDescent="0.2">
-      <c r="A147" s="182"/>
-      <c r="B147" s="185"/>
+      <c r="A147" s="168"/>
+      <c r="B147" s="171"/>
       <c r="C147" s="136" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D147" s="51"/>
       <c r="E147" s="4" t="s">
         <v>173</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="148" spans="1:59" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="183"/>
-      <c r="B148" s="186"/>
+      <c r="A148" s="169"/>
+      <c r="B148" s="172"/>
       <c r="C148" s="55"/>
       <c r="D148" s="55"/>
       <c r="E148" s="117"/>
@@ -6287,19 +6289,19 @@
     <row r="153" spans="1:59" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="8"/>
       <c r="C153" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="154" spans="1:59" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="8"/>
       <c r="C154" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="155" spans="1:59" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="8"/>
       <c r="C155" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="156" spans="1:59" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -6401,6 +6403,59 @@
     <row r="250" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="B41:B56"/>
+    <mergeCell ref="A41:A56"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="A120:A126"/>
+    <mergeCell ref="B120:B126"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="A135:A140"/>
+    <mergeCell ref="B135:B140"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="A102:A107"/>
+    <mergeCell ref="B102:B107"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="A57:A70"/>
+    <mergeCell ref="B57:B70"/>
     <mergeCell ref="A146:A148"/>
     <mergeCell ref="B146:B148"/>
     <mergeCell ref="D3:D4"/>
@@ -6417,59 +6472,6 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="A102:A107"/>
-    <mergeCell ref="B102:B107"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="A57:A70"/>
-    <mergeCell ref="B57:B70"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="B143:B145"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="B132:B134"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="A135:A140"/>
-    <mergeCell ref="B135:B140"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="A120:A126"/>
-    <mergeCell ref="B120:B126"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="A110:A113"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="B41:B56"/>
-    <mergeCell ref="A41:A56"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="4" orientation="portrait" r:id="rId1"/>
@@ -6497,19 +6499,19 @@
     </row>
     <row r="2" spans="1:6" s="39" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="198" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="197" t="s">
+      <c r="C3" s="198" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="197" t="s">
+      <c r="D3" s="198" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="197" t="s">
+      <c r="E3" s="198" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="101" t="s">
@@ -6517,11 +6519,11 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="198"/>
+      <c r="A4" s="199"/>
       <c r="B4" s="201"/>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="198"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="199"/>
       <c r="F4" s="102" t="s">
         <v>6</v>
       </c>
@@ -6530,10 +6532,10 @@
       <c r="A5" s="195">
         <v>2.1</v>
       </c>
-      <c r="B5" s="167" t="s">
+      <c r="B5" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="180" t="s">
         <v>137</v>
       </c>
       <c r="D5" s="23"/>
@@ -6541,9 +6543,9 @@
       <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="196"/>
-      <c r="B6" s="169"/>
-      <c r="C6" s="171"/>
+      <c r="A6" s="197"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="181"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
@@ -6552,7 +6554,7 @@
       <c r="A7" s="195">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B7" s="167" t="s">
+      <c r="B7" s="175" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="3"/>
@@ -6561,8 +6563,8 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="199"/>
-      <c r="B8" s="168"/>
+      <c r="A8" s="196"/>
+      <c r="B8" s="176"/>
       <c r="C8" s="3" t="s">
         <v>55</v>
       </c>
@@ -6573,8 +6575,8 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="199"/>
-      <c r="B9" s="168"/>
+      <c r="A9" s="196"/>
+      <c r="B9" s="176"/>
       <c r="C9" s="3" t="s">
         <v>56</v>
       </c>
@@ -6585,8 +6587,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="199"/>
-      <c r="B10" s="168"/>
+      <c r="A10" s="196"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="3" t="s">
         <v>57</v>
       </c>
@@ -6599,8 +6601,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="199"/>
-      <c r="B11" s="168"/>
+      <c r="A11" s="196"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="3" t="s">
         <v>58</v>
       </c>
@@ -6611,8 +6613,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="199"/>
-      <c r="B12" s="168"/>
+      <c r="A12" s="196"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="3" t="s">
         <v>59</v>
       </c>
@@ -6623,8 +6625,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="199"/>
-      <c r="B13" s="168"/>
+      <c r="A13" s="196"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="3" t="s">
         <v>60</v>
       </c>
@@ -6635,8 +6637,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="199"/>
-      <c r="B14" s="168"/>
+      <c r="A14" s="196"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="3" t="s">
         <v>62</v>
       </c>
@@ -6647,8 +6649,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="199"/>
-      <c r="B15" s="168"/>
+      <c r="A15" s="196"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="3" t="s">
         <v>104</v>
       </c>
@@ -6657,8 +6659,8 @@
       <c r="F15" s="83"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="199"/>
-      <c r="B16" s="168"/>
+      <c r="A16" s="196"/>
+      <c r="B16" s="176"/>
       <c r="C16" s="3" t="s">
         <v>105</v>
       </c>
@@ -6669,8 +6671,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="199"/>
-      <c r="B17" s="168"/>
+      <c r="A17" s="196"/>
+      <c r="B17" s="176"/>
       <c r="C17" s="3" t="s">
         <v>106</v>
       </c>
@@ -6681,8 +6683,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="199"/>
-      <c r="B18" s="168"/>
+      <c r="A18" s="196"/>
+      <c r="B18" s="176"/>
       <c r="C18" s="3" t="s">
         <v>107</v>
       </c>
@@ -6693,13 +6695,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="199"/>
-      <c r="B19" s="168"/>
+      <c r="A19" s="196"/>
+      <c r="B19" s="176"/>
       <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E19" s="63"/>
       <c r="F19" s="4" t="s">
@@ -6707,8 +6709,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="199"/>
-      <c r="B20" s="168"/>
+      <c r="A20" s="196"/>
+      <c r="B20" s="176"/>
       <c r="C20" s="63"/>
       <c r="D20" s="3" t="s">
         <v>108</v>
@@ -6719,8 +6721,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="196"/>
-      <c r="B21" s="169"/>
+      <c r="A21" s="197"/>
+      <c r="B21" s="179"/>
       <c r="C21" s="56"/>
       <c r="D21" s="29" t="s">
         <v>109</v>
@@ -6734,8 +6736,8 @@
       <c r="A22" s="195">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B22" s="167" t="s">
-        <v>311</v>
+      <c r="B22" s="175" t="s">
+        <v>310</v>
       </c>
       <c r="C22" s="82"/>
       <c r="D22" s="54"/>
@@ -6743,10 +6745,10 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="199"/>
-      <c r="B23" s="168"/>
+      <c r="A23" s="196"/>
+      <c r="B23" s="176"/>
       <c r="C23" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D23" s="57"/>
       <c r="E23" s="4" t="s">
@@ -6755,8 +6757,8 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="199"/>
-      <c r="B24" s="168"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="176"/>
       <c r="C24" s="3" t="s">
         <v>56</v>
       </c>
@@ -6767,8 +6769,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="199"/>
-      <c r="B25" s="168"/>
+      <c r="A25" s="196"/>
+      <c r="B25" s="176"/>
       <c r="C25" s="3" t="s">
         <v>57</v>
       </c>
@@ -6781,8 +6783,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="199"/>
-      <c r="B26" s="168"/>
+      <c r="A26" s="196"/>
+      <c r="B26" s="176"/>
       <c r="C26" s="3" t="s">
         <v>58</v>
       </c>
@@ -6795,8 +6797,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="199"/>
-      <c r="B27" s="168"/>
+      <c r="A27" s="196"/>
+      <c r="B27" s="176"/>
       <c r="C27" s="3" t="s">
         <v>59</v>
       </c>
@@ -6807,8 +6809,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="199"/>
-      <c r="B28" s="168"/>
+      <c r="A28" s="196"/>
+      <c r="B28" s="176"/>
       <c r="C28" s="3" t="s">
         <v>60</v>
       </c>
@@ -6819,8 +6821,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="196"/>
-      <c r="B29" s="169"/>
+      <c r="A29" s="197"/>
+      <c r="B29" s="179"/>
       <c r="C29" s="29" t="s">
         <v>138</v>
       </c>
@@ -6834,7 +6836,7 @@
       <c r="A30" s="195">
         <v>2.4</v>
       </c>
-      <c r="B30" s="167" t="s">
+      <c r="B30" s="175" t="s">
         <v>63</v>
       </c>
       <c r="C30" s="54"/>
@@ -6843,8 +6845,8 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="199"/>
-      <c r="B31" s="168"/>
+      <c r="A31" s="196"/>
+      <c r="B31" s="176"/>
       <c r="C31" s="50" t="s">
         <v>16</v>
       </c>
@@ -6857,8 +6859,8 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="199"/>
-      <c r="B32" s="168"/>
+      <c r="A32" s="196"/>
+      <c r="B32" s="176"/>
       <c r="C32" s="50"/>
       <c r="D32" s="3" t="s">
         <v>56</v>
@@ -6869,8 +6871,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="199"/>
-      <c r="B33" s="168"/>
+      <c r="A33" s="196"/>
+      <c r="B33" s="176"/>
       <c r="C33" s="50"/>
       <c r="D33" s="3" t="s">
         <v>57</v>
@@ -6879,12 +6881,12 @@
         <v>174</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="199"/>
-      <c r="B34" s="168"/>
+      <c r="A34" s="196"/>
+      <c r="B34" s="176"/>
       <c r="C34" s="50"/>
       <c r="D34" s="3" t="s">
         <v>58</v>
@@ -6895,8 +6897,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="199"/>
-      <c r="B35" s="168"/>
+      <c r="A35" s="196"/>
+      <c r="B35" s="176"/>
       <c r="C35" s="50"/>
       <c r="D35" s="3" t="s">
         <v>59</v>
@@ -6907,8 +6909,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="199"/>
-      <c r="B36" s="168"/>
+      <c r="A36" s="196"/>
+      <c r="B36" s="176"/>
       <c r="C36" s="50"/>
       <c r="D36" s="3" t="s">
         <v>60</v>
@@ -6919,8 +6921,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="196"/>
-      <c r="B37" s="169"/>
+      <c r="A37" s="197"/>
+      <c r="B37" s="179"/>
       <c r="C37" s="30"/>
       <c r="D37" s="29" t="s">
         <v>62</v>
@@ -6931,10 +6933,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="167">
+      <c r="A38" s="175">
         <v>2.5</v>
       </c>
-      <c r="B38" s="167" t="s">
+      <c r="B38" s="175" t="s">
         <v>197</v>
       </c>
       <c r="C38" s="54"/>
@@ -6943,8 +6945,8 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="168"/>
-      <c r="B39" s="168"/>
+      <c r="A39" s="176"/>
+      <c r="B39" s="176"/>
       <c r="C39" s="50"/>
       <c r="D39" s="3" t="s">
         <v>198</v>
@@ -6954,8 +6956,8 @@
       <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="168"/>
-      <c r="B40" s="168"/>
+      <c r="A40" s="176"/>
+      <c r="B40" s="176"/>
       <c r="C40" s="50"/>
       <c r="D40" s="3" t="s">
         <v>56</v>
@@ -6966,8 +6968,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="168"/>
-      <c r="B41" s="168"/>
+      <c r="A41" s="176"/>
+      <c r="B41" s="176"/>
       <c r="C41" s="50"/>
       <c r="D41" s="3" t="s">
         <v>57</v>
@@ -6979,8 +6981,8 @@
       <c r="G41" s="43"/>
     </row>
     <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="168"/>
-      <c r="B42" s="168"/>
+      <c r="A42" s="176"/>
+      <c r="B42" s="176"/>
       <c r="C42" s="50"/>
       <c r="D42" s="3" t="s">
         <v>65</v>
@@ -6991,8 +6993,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="168"/>
-      <c r="B43" s="168"/>
+      <c r="A43" s="176"/>
+      <c r="B43" s="176"/>
       <c r="C43" s="50"/>
       <c r="D43" s="3" t="s">
         <v>58</v>
@@ -7003,8 +7005,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="168"/>
-      <c r="B44" s="168"/>
+      <c r="A44" s="176"/>
+      <c r="B44" s="176"/>
       <c r="C44" s="50"/>
       <c r="D44" s="3" t="s">
         <v>59</v>
@@ -7015,8 +7017,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="168"/>
-      <c r="B45" s="168"/>
+      <c r="A45" s="176"/>
+      <c r="B45" s="176"/>
       <c r="C45" s="50"/>
       <c r="D45" s="3" t="s">
         <v>60</v>
@@ -7027,8 +7029,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="169"/>
-      <c r="B46" s="169"/>
+      <c r="A46" s="179"/>
+      <c r="B46" s="179"/>
       <c r="C46" s="30"/>
       <c r="D46" s="29" t="s">
         <v>62</v>
@@ -7039,11 +7041,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="167">
+      <c r="A47" s="175">
         <v>2.6</v>
       </c>
-      <c r="B47" s="167" t="s">
-        <v>313</v>
+      <c r="B47" s="175" t="s">
+        <v>312</v>
       </c>
       <c r="C47" s="54"/>
       <c r="D47" s="82"/>
@@ -7051,18 +7053,18 @@
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="168"/>
-      <c r="B48" s="168"/>
+      <c r="A48" s="176"/>
+      <c r="B48" s="176"/>
       <c r="C48" s="50"/>
       <c r="D48" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E48" s="51"/>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="168"/>
-      <c r="B49" s="168"/>
+      <c r="A49" s="176"/>
+      <c r="B49" s="176"/>
       <c r="C49" s="50"/>
       <c r="D49" s="3" t="s">
         <v>56</v>
@@ -7073,8 +7075,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="168"/>
-      <c r="B50" s="168"/>
+      <c r="A50" s="176"/>
+      <c r="B50" s="176"/>
       <c r="C50" s="50"/>
       <c r="D50" s="3" t="s">
         <v>57</v>
@@ -7086,8 +7088,8 @@
       <c r="H50" s="43"/>
     </row>
     <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="168"/>
-      <c r="B51" s="168"/>
+      <c r="A51" s="176"/>
+      <c r="B51" s="176"/>
       <c r="C51" s="50"/>
       <c r="D51" s="3" t="s">
         <v>58</v>
@@ -7098,8 +7100,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="168"/>
-      <c r="B52" s="168"/>
+      <c r="A52" s="176"/>
+      <c r="B52" s="176"/>
       <c r="C52" s="50"/>
       <c r="D52" s="3" t="s">
         <v>59</v>
@@ -7110,8 +7112,8 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="168"/>
-      <c r="B53" s="168"/>
+      <c r="A53" s="176"/>
+      <c r="B53" s="176"/>
       <c r="C53" s="50"/>
       <c r="D53" s="3" t="s">
         <v>60</v>
@@ -7122,8 +7124,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="168"/>
-      <c r="B54" s="168"/>
+      <c r="A54" s="176"/>
+      <c r="B54" s="176"/>
       <c r="C54" s="50"/>
       <c r="D54" s="3" t="s">
         <v>62</v>
@@ -7134,11 +7136,11 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="168"/>
-      <c r="B55" s="168"/>
+      <c r="A55" s="176"/>
+      <c r="B55" s="176"/>
       <c r="C55" s="50"/>
       <c r="D55" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E55" s="51" t="s">
         <v>193</v>
@@ -7148,11 +7150,11 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="178">
+      <c r="A56" s="186">
         <v>2.7</v>
       </c>
-      <c r="B56" s="187" t="s">
-        <v>316</v>
+      <c r="B56" s="188" t="s">
+        <v>315</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="77"/>
@@ -7160,18 +7162,18 @@
       <c r="F56" s="33"/>
     </row>
     <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="179"/>
-      <c r="B57" s="168"/>
+      <c r="A57" s="192"/>
+      <c r="B57" s="176"/>
       <c r="C57" s="50"/>
       <c r="D57" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E57" s="51"/>
       <c r="F57" s="61"/>
     </row>
     <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="179"/>
-      <c r="B58" s="168"/>
+      <c r="A58" s="192"/>
+      <c r="B58" s="176"/>
       <c r="C58" s="50"/>
       <c r="D58" s="3" t="s">
         <v>56</v>
@@ -7182,8 +7184,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="179"/>
-      <c r="B59" s="168"/>
+      <c r="A59" s="192"/>
+      <c r="B59" s="176"/>
       <c r="C59" s="50"/>
       <c r="D59" s="3" t="s">
         <v>57</v>
@@ -7197,8 +7199,8 @@
       <c r="H59" s="43"/>
     </row>
     <row r="60" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="179"/>
-      <c r="B60" s="168"/>
+      <c r="A60" s="192"/>
+      <c r="B60" s="176"/>
       <c r="C60" s="50"/>
       <c r="D60" s="3" t="s">
         <v>58</v>
@@ -7209,8 +7211,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="179"/>
-      <c r="B61" s="168"/>
+      <c r="A61" s="192"/>
+      <c r="B61" s="176"/>
       <c r="C61" s="50"/>
       <c r="D61" s="3" t="s">
         <v>59</v>
@@ -7221,8 +7223,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="179"/>
-      <c r="B62" s="168"/>
+      <c r="A62" s="192"/>
+      <c r="B62" s="176"/>
       <c r="C62" s="50"/>
       <c r="D62" s="3" t="s">
         <v>60</v>
@@ -7233,8 +7235,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="180"/>
-      <c r="B63" s="188"/>
+      <c r="A63" s="187"/>
+      <c r="B63" s="189"/>
       <c r="C63" s="35"/>
       <c r="D63" s="78" t="s">
         <v>62</v>
@@ -7246,6 +7248,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A22:A29"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="A56:A63"/>
     <mergeCell ref="B56:B63"/>
     <mergeCell ref="A47:A55"/>
@@ -7256,16 +7268,6 @@
     <mergeCell ref="B38:B46"/>
     <mergeCell ref="A30:A37"/>
     <mergeCell ref="B30:B37"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="B22:B29"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7300,19 +7302,19 @@
     </row>
     <row r="2" spans="1:7" s="39" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="189" t="s">
+      <c r="C3" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="189" t="s">
+      <c r="D3" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="189" t="s">
+      <c r="E3" s="173" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -7320,17 +7322,17 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="202"/>
-      <c r="B4" s="205"/>
-      <c r="C4" s="202"/>
-      <c r="D4" s="202"/>
-      <c r="E4" s="202"/>
+      <c r="A4" s="208"/>
+      <c r="B4" s="209"/>
+      <c r="C4" s="208"/>
+      <c r="D4" s="208"/>
+      <c r="E4" s="208"/>
       <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="178">
+      <c r="A5" s="186">
         <v>3.1</v>
       </c>
       <c r="B5" s="203" t="s">
@@ -7342,8 +7344,8 @@
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="179"/>
-      <c r="B6" s="173"/>
+      <c r="A6" s="192"/>
+      <c r="B6" s="178"/>
       <c r="C6" s="49" t="s">
         <v>128</v>
       </c>
@@ -7351,30 +7353,30 @@
       <c r="F6" s="61"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="179"/>
-      <c r="B7" s="173"/>
+      <c r="A7" s="192"/>
+      <c r="B7" s="178"/>
       <c r="C7" s="49" t="s">
         <v>129</v>
       </c>
       <c r="E7" s="66"/>
       <c r="F7" s="104" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="179"/>
-      <c r="B8" s="173"/>
+      <c r="A8" s="192"/>
+      <c r="B8" s="178"/>
       <c r="C8" s="49" t="s">
         <v>130</v>
       </c>
       <c r="E8" s="66"/>
       <c r="F8" s="61" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="179"/>
-      <c r="B9" s="173"/>
+      <c r="A9" s="192"/>
+      <c r="B9" s="178"/>
       <c r="C9" s="67" t="s">
         <v>254</v>
       </c>
@@ -7387,8 +7389,8 @@
       <c r="G9" s="134"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="179"/>
-      <c r="B10" s="173"/>
+      <c r="A10" s="192"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="49" t="s">
         <v>131</v>
       </c>
@@ -7398,8 +7400,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="179"/>
-      <c r="B11" s="173"/>
+      <c r="A11" s="192"/>
+      <c r="B11" s="178"/>
       <c r="C11" s="106" t="s">
         <v>217</v>
       </c>
@@ -7409,8 +7411,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="179"/>
-      <c r="B12" s="173"/>
+      <c r="A12" s="192"/>
+      <c r="B12" s="178"/>
       <c r="C12" s="106" t="s">
         <v>218</v>
       </c>
@@ -7420,8 +7422,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="179"/>
-      <c r="B13" s="173"/>
+      <c r="A13" s="192"/>
+      <c r="B13" s="178"/>
       <c r="C13" s="106" t="s">
         <v>219</v>
       </c>
@@ -7431,8 +7433,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="179"/>
-      <c r="B14" s="173"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="178"/>
       <c r="C14" s="106" t="s">
         <v>220</v>
       </c>
@@ -7442,8 +7444,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="179"/>
-      <c r="B15" s="173"/>
+      <c r="A15" s="192"/>
+      <c r="B15" s="178"/>
       <c r="C15" s="107" t="s">
         <v>221</v>
       </c>
@@ -7453,7 +7455,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="180"/>
+      <c r="A16" s="187"/>
       <c r="B16" s="204"/>
       <c r="C16" s="121"/>
       <c r="D16" s="119"/>
@@ -7461,10 +7463,10 @@
       <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="179">
+      <c r="A17" s="192">
         <v>3.2</v>
       </c>
-      <c r="B17" s="173" t="s">
+      <c r="B17" s="178" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="67"/>
@@ -7475,8 +7477,8 @@
       <c r="F17" s="61"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="179"/>
-      <c r="B18" s="173"/>
+      <c r="A18" s="192"/>
+      <c r="B18" s="178"/>
       <c r="C18" s="67" t="s">
         <v>281</v>
       </c>
@@ -7485,8 +7487,8 @@
       <c r="F18" s="61"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="179"/>
-      <c r="B19" s="173"/>
+      <c r="A19" s="192"/>
+      <c r="B19" s="178"/>
       <c r="C19" s="67" t="s">
         <v>282</v>
       </c>
@@ -7499,8 +7501,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="206"/>
-      <c r="B20" s="174"/>
+      <c r="A20" s="202"/>
+      <c r="B20" s="194"/>
       <c r="C20" s="70" t="s">
         <v>283</v>
       </c>
@@ -7513,11 +7515,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="178">
+      <c r="A21" s="186">
         <v>3.3</v>
       </c>
       <c r="B21" s="203" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="103"/>
@@ -7525,8 +7527,8 @@
       <c r="F21" s="33"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="179"/>
-      <c r="B22" s="173"/>
+      <c r="A22" s="192"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="67"/>
       <c r="D22" s="40" t="s">
         <v>215</v>
@@ -7537,8 +7539,8 @@
       <c r="F22" s="61"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="179"/>
-      <c r="B23" s="173"/>
+      <c r="A23" s="192"/>
+      <c r="B23" s="178"/>
       <c r="C23" s="67"/>
       <c r="D23" s="40" t="s">
         <v>284</v>
@@ -7551,8 +7553,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="179"/>
-      <c r="B24" s="173"/>
+      <c r="A24" s="192"/>
+      <c r="B24" s="178"/>
       <c r="C24" s="67"/>
       <c r="D24" s="40" t="s">
         <v>285</v>
@@ -7565,7 +7567,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="180"/>
+      <c r="A25" s="187"/>
       <c r="B25" s="204"/>
       <c r="C25" s="70"/>
       <c r="D25" s="110" t="s">
@@ -7579,11 +7581,11 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="178">
+      <c r="A26" s="186">
         <v>3.4</v>
       </c>
-      <c r="B26" s="207" t="s">
-        <v>320</v>
+      <c r="B26" s="205" t="s">
+        <v>319</v>
       </c>
       <c r="C26" s="87"/>
       <c r="D26" s="87"/>
@@ -7591,96 +7593,96 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="179"/>
-      <c r="B27" s="208"/>
+      <c r="A27" s="192"/>
+      <c r="B27" s="206"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E27" s="66"/>
       <c r="F27" s="61"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="179"/>
-      <c r="B28" s="208"/>
+      <c r="A28" s="192"/>
+      <c r="B28" s="206"/>
       <c r="C28" s="49"/>
       <c r="D28" s="49" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E28" s="66"/>
       <c r="F28" s="104" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="179"/>
-      <c r="B29" s="208"/>
+      <c r="A29" s="192"/>
+      <c r="B29" s="206"/>
       <c r="C29" s="49"/>
       <c r="D29" s="107" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E29" s="66" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F29" s="61"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="179"/>
-      <c r="B30" s="208"/>
+      <c r="A30" s="192"/>
+      <c r="B30" s="206"/>
       <c r="C30" s="49"/>
       <c r="D30" s="107" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E30" s="66" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F30" s="108" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="179"/>
-      <c r="B31" s="208"/>
+      <c r="A31" s="192"/>
+      <c r="B31" s="206"/>
       <c r="C31" s="49"/>
       <c r="D31" s="107" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E31" s="66" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F31" s="108" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="179"/>
-      <c r="B32" s="208"/>
+      <c r="A32" s="192"/>
+      <c r="B32" s="206"/>
       <c r="C32" s="49"/>
       <c r="D32" s="107" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E32" s="66" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F32" s="108" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="179"/>
-      <c r="B33" s="208"/>
+      <c r="A33" s="192"/>
+      <c r="B33" s="206"/>
       <c r="C33" s="49"/>
       <c r="D33" s="49" t="s">
         <v>130</v>
       </c>
       <c r="E33" s="137"/>
       <c r="F33" s="104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="179"/>
-      <c r="B34" s="208"/>
+      <c r="A34" s="192"/>
+      <c r="B34" s="206"/>
       <c r="C34" s="49"/>
       <c r="D34" s="49" t="s">
         <v>131</v>
@@ -7691,8 +7693,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="179"/>
-      <c r="B35" s="208"/>
+      <c r="A35" s="192"/>
+      <c r="B35" s="206"/>
       <c r="C35" s="106"/>
       <c r="D35" s="106" t="s">
         <v>217</v>
@@ -7703,8 +7705,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="179"/>
-      <c r="B36" s="208"/>
+      <c r="A36" s="192"/>
+      <c r="B36" s="206"/>
       <c r="C36" s="106"/>
       <c r="D36" s="106" t="s">
         <v>218</v>
@@ -7715,8 +7717,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="179"/>
-      <c r="B37" s="208"/>
+      <c r="A37" s="192"/>
+      <c r="B37" s="206"/>
       <c r="C37" s="106"/>
       <c r="D37" s="106" t="s">
         <v>219</v>
@@ -7727,8 +7729,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="179"/>
-      <c r="B38" s="208"/>
+      <c r="A38" s="192"/>
+      <c r="B38" s="206"/>
       <c r="C38" s="106"/>
       <c r="D38" s="106" t="s">
         <v>220</v>
@@ -7739,8 +7741,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="179"/>
-      <c r="B39" s="208"/>
+      <c r="A39" s="192"/>
+      <c r="B39" s="206"/>
       <c r="C39" s="107"/>
       <c r="D39" s="107" t="s">
         <v>221</v>
@@ -7751,16 +7753,16 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="179"/>
-      <c r="B40" s="208"/>
+      <c r="A40" s="192"/>
+      <c r="B40" s="206"/>
       <c r="C40" s="107"/>
       <c r="D40" s="107"/>
       <c r="E40" s="66"/>
       <c r="F40" s="108"/>
     </row>
     <row r="41" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="180"/>
-      <c r="B41" s="209"/>
+      <c r="A41" s="187"/>
+      <c r="B41" s="207"/>
       <c r="C41" s="121"/>
       <c r="D41" s="121"/>
       <c r="E41" s="116"/>
@@ -7957,12 +7959,6 @@
     <row r="230" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="A26:A41"/>
-    <mergeCell ref="B26:B41"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="A5:A16"/>
@@ -7970,6 +7966,12 @@
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="A26:A41"/>
+    <mergeCell ref="B26:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8002,19 +8004,19 @@
     </row>
     <row r="2" spans="1:18" s="39" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="189" t="s">
+      <c r="C3" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="189" t="s">
+      <c r="D3" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="189" t="s">
+      <c r="E3" s="173" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -8022,20 +8024,20 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="190"/>
-      <c r="B4" s="194"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
+      <c r="A4" s="174"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="174"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="167">
+      <c r="A5" s="175">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B5" s="167" t="s">
+      <c r="B5" s="175" t="s">
         <v>69</v>
       </c>
       <c r="C5" s="46"/>
@@ -8046,8 +8048,8 @@
       <c r="F5" s="111"/>
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="168"/>
-      <c r="B6" s="168"/>
+      <c r="A6" s="176"/>
+      <c r="B6" s="176"/>
       <c r="C6" s="57"/>
       <c r="D6" s="3" t="s">
         <v>70</v>
@@ -8060,11 +8062,11 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="168"/>
-      <c r="B7" s="168"/>
+      <c r="A7" s="176"/>
+      <c r="B7" s="176"/>
       <c r="C7" s="58"/>
       <c r="D7" s="35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E7" s="36"/>
       <c r="F7" s="112" t="s">
@@ -8072,11 +8074,11 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="167">
+      <c r="A8" s="175">
         <v>4.2</v>
       </c>
-      <c r="B8" s="167" t="s">
-        <v>322</v>
+      <c r="B8" s="175" t="s">
+        <v>321</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="72"/>
@@ -8098,10 +8100,10 @@
       <c r="R8" s="211"/>
     </row>
     <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="168"/>
-      <c r="B9" s="168"/>
+      <c r="A9" s="176"/>
+      <c r="B9" s="176"/>
       <c r="C9" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
@@ -8120,22 +8122,22 @@
       <c r="R9" s="211"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="168"/>
-      <c r="B10" s="168"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="3"/>
       <c r="D10" s="72"/>
       <c r="E10" s="128"/>
       <c r="F10" s="127"/>
     </row>
     <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="168"/>
-      <c r="B11" s="168"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D11" s="72"/>
       <c r="E11" s="135" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F11" s="130" t="s">
         <v>139</v>
@@ -8149,11 +8151,11 @@
       <c r="M11" s="125"/>
     </row>
     <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="168"/>
-      <c r="B12" s="168"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="3"/>
       <c r="D12" s="50" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E12" s="129"/>
       <c r="F12" s="131" t="s">
@@ -8168,14 +8170,14 @@
       <c r="M12" s="125"/>
     </row>
     <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="168"/>
-      <c r="B13" s="168"/>
+      <c r="A13" s="176"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="3" t="s">
         <v>225</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="135" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F13" s="130" t="s">
         <v>139</v>
@@ -8189,8 +8191,8 @@
       <c r="M13" s="125"/>
     </row>
     <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="168"/>
-      <c r="B14" s="168"/>
+      <c r="A14" s="176"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="63"/>
       <c r="D14" s="50" t="s">
         <v>226</v>
@@ -8201,18 +8203,18 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="169"/>
-      <c r="B15" s="169"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="179"/>
       <c r="C15" s="56"/>
       <c r="D15" s="29"/>
       <c r="E15" s="88"/>
       <c r="F15" s="89"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="167">
+      <c r="A16" s="175">
         <v>4.3</v>
       </c>
-      <c r="B16" s="167" t="s">
+      <c r="B16" s="175" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="85"/>
@@ -8221,8 +8223,8 @@
       <c r="F16" s="72"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="168"/>
-      <c r="B17" s="168"/>
+      <c r="A17" s="176"/>
+      <c r="B17" s="176"/>
       <c r="C17" s="3" t="s">
         <v>72</v>
       </c>
@@ -8233,8 +8235,8 @@
       <c r="F17" s="72"/>
     </row>
     <row r="18" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="168"/>
-      <c r="B18" s="168"/>
+      <c r="A18" s="176"/>
+      <c r="B18" s="176"/>
       <c r="C18" s="3" t="s">
         <v>248</v>
       </c>
@@ -8247,8 +8249,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="168"/>
-      <c r="B19" s="168"/>
+      <c r="A19" s="176"/>
+      <c r="B19" s="176"/>
       <c r="C19" s="3" t="s">
         <v>249</v>
       </c>
@@ -8261,8 +8263,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="168"/>
-      <c r="B20" s="168"/>
+      <c r="A20" s="176"/>
+      <c r="B20" s="176"/>
       <c r="C20" s="90" t="s">
         <v>250</v>
       </c>
@@ -8275,8 +8277,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="168"/>
-      <c r="B21" s="168"/>
+      <c r="A21" s="176"/>
+      <c r="B21" s="176"/>
       <c r="C21" s="91" t="s">
         <v>251</v>
       </c>
@@ -8290,8 +8292,8 @@
       <c r="G21" s="115"/>
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="168"/>
-      <c r="B22" s="168"/>
+      <c r="A22" s="176"/>
+      <c r="B22" s="176"/>
       <c r="C22" s="91"/>
       <c r="D22" s="3" t="s">
         <v>228</v>
@@ -8304,8 +8306,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="169"/>
-      <c r="B23" s="169"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="179"/>
       <c r="C23" s="3"/>
       <c r="D23" s="29" t="s">
         <v>232</v>
@@ -8318,10 +8320,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="191">
+      <c r="A24" s="182">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B24" s="191" t="s">
+      <c r="B24" s="182" t="s">
         <v>73</v>
       </c>
       <c r="C24" s="215" t="s">
@@ -8652,13 +8654,6 @@
     <row r="324" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
     <mergeCell ref="G8:R9"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="A24:A25"/>
@@ -8670,6 +8665,13 @@
     <mergeCell ref="B16:B23"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="4" orientation="portrait" r:id="rId1"/>

</xml_diff>